<commit_message>
changes states names deleted flattened sheet
</commit_message>
<xml_diff>
--- a/arrivals_departures_by_state.xlsx
+++ b/arrivals_departures_by_state.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" updateLinks="never" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E7380A-A7D0-4BC3-8BD5-360FE450E20A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A03F52-5E2B-4E87-9C12-1BC759A4E1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2985" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="742" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,37 +72,105 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="8">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="17"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="31"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="44"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="58"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="74"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="88"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="101"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="8">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+    <bk>
+      <rc t="1" v="1"/>
+    </bk>
+    <bk>
+      <rc t="1" v="2"/>
+    </bk>
+    <bk>
+      <rc t="1" v="3"/>
+    </bk>
+    <bk>
+      <rc t="1" v="4"/>
+    </bk>
+    <bk>
+      <rc t="1" v="5"/>
+    </bk>
+    <bk>
+      <rc t="1" v="6"/>
+    </bk>
+    <bk>
+      <rc t="1" v="7"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>ACT</t>
-  </si>
-  <si>
-    <t>NSW</t>
-  </si>
-  <si>
-    <t>Vic.</t>
-  </si>
-  <si>
-    <t>SA</t>
-  </si>
-  <si>
-    <t>WA</t>
-  </si>
-  <si>
-    <t>Tas.</t>
-  </si>
-  <si>
-    <t>NT</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Year</t>
   </si>
   <si>
     <t>State</t>
-  </si>
-  <si>
-    <t>QLD</t>
   </si>
   <si>
     <t>Departures</t>
@@ -693,13 +761,12 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="45" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="62">
@@ -845,6 +912,1662 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+  <types>
+    <type name="_linkedentity2">
+      <keyFlags>
+        <key name="%EntityServiceId">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%EntityCulture">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%EntityId">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%cvi">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+          <flag name="ExcludeFromCalcComparison" value="1"/>
+        </key>
+      </keyFlags>
+    </type>
+    <type name="_linkedentity2core">
+      <keyFlags>
+        <key name="%EntityServiceId">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%EntityCulture">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%EntityId">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%IsRefreshable">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+          <flag name="ExcludeFromCalcComparison" value="1"/>
+        </key>
+        <key name="%ProviderInfo">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%DataProviderExternalLinkLogo">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%DataProviderExternalLink">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%DataRetrievedTime">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+          <flag name="ExcludeFromCalcComparison" value="1"/>
+        </key>
+        <key name="%EntityDomainIdString">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%InfoToolTipLabelNames">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%InfoToolTipLabelValues">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%InfoToolTipLabelValuesType">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%DataProviderString">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%ClassificationId">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%OutdatedReason">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+          <flag name="ExcludeFromCalcComparison" value="1"/>
+        </key>
+      </keyFlags>
+    </type>
+    <type name="_webimage">
+      <keyFlags>
+        <key name="WebImageIdentifier">
+          <flag name="ShowInCardView" value="0"/>
+        </key>
+      </keyFlags>
+    </type>
+  </types>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdRichValueWebImage.xml><?xml version="1.0" encoding="utf-8"?>
+<webImagesSrd xmlns="http://schemas.microsoft.com/office/spreadsheetml/2020/richdatawebimage" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <webImageSrd>
+    <address r:id="rId1"/>
+    <moreImagesAddress r:id="rId2"/>
+  </webImageSrd>
+  <webImageSrd>
+    <address r:id="rId3"/>
+    <moreImagesAddress r:id="rId4"/>
+  </webImageSrd>
+  <webImageSrd>
+    <address r:id="rId5"/>
+    <moreImagesAddress r:id="rId6"/>
+  </webImageSrd>
+  <webImageSrd>
+    <address r:id="rId7"/>
+    <moreImagesAddress r:id="rId8"/>
+  </webImageSrd>
+  <webImageSrd>
+    <address r:id="rId9"/>
+    <moreImagesAddress r:id="rId10"/>
+  </webImageSrd>
+  <webImageSrd>
+    <address r:id="rId11"/>
+    <moreImagesAddress r:id="rId12"/>
+  </webImageSrd>
+  <webImageSrd>
+    <address r:id="rId13"/>
+    <moreImagesAddress r:id="rId14"/>
+  </webImageSrd>
+  <webImageSrd>
+    <address r:id="rId15"/>
+    <moreImagesAddress r:id="rId16"/>
+  </webImageSrd>
+</webImagesSrd>
+</file>
+
+<file path=xl/richData/rdarray.xml><?xml version="1.0" encoding="utf-8"?>
+<arrayData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="8">
+  <a r="4">
+    <v t="r">6</v>
+    <v t="r">6</v>
+    <v t="r">7</v>
+    <v t="r">8</v>
+  </a>
+  <a r="4">
+    <v t="r">6</v>
+    <v t="r">6</v>
+    <v t="r">22</v>
+    <v t="r">23</v>
+  </a>
+  <a r="4">
+    <v t="r">6</v>
+    <v t="r">6</v>
+    <v t="r">36</v>
+    <v t="r">37</v>
+  </a>
+  <a r="4">
+    <v t="r">6</v>
+    <v t="r">6</v>
+    <v t="r">49</v>
+    <v t="r">50</v>
+  </a>
+  <a r="4">
+    <v t="r">6</v>
+    <v t="r">6</v>
+    <v t="r">64</v>
+    <v t="r">65</v>
+  </a>
+  <a r="4">
+    <v t="r">6</v>
+    <v t="r">6</v>
+    <v t="r">79</v>
+    <v t="r">80</v>
+  </a>
+  <a r="1">
+    <v t="r">93</v>
+  </a>
+  <a r="1">
+    <v t="r">106</v>
+  </a>
+</arrayData>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="115">
+  <rv s="0">
+    <v>536870912</v>
+    <v>New South Wales</v>
+    <v>9143b1e4-782f-52c3-0f4a-cea5eaf6f36a</v>
+    <v>en-AU</v>
+    <v>Map</v>
+  </rv>
+  <rv s="1">
+    <fb>801150</fb>
+    <v>11</v>
+  </rv>
+  <rv s="0">
+    <v>536870912</v>
+    <v>Sydney</v>
+    <v>3ecec2e8-2993-42e7-7299-f693bbe3b9b9</v>
+    <v>en-AU</v>
+    <v>Map</v>
+  </rv>
+  <rv s="0">
+    <v>536870912</v>
+    <v>Australia</v>
+    <v>06de2191-243d-a83f-6990-2eb1c7f3382a</v>
+    <v>en-AU</v>
+    <v>Map</v>
+  </rv>
+  <rv s="1">
+    <fb>2604314</fb>
+    <v>11</v>
+  </rv>
+  <rv s="2">
+    <v>0</v>
+    <v>9</v>
+    <v>0</v>
+    <v>7</v>
+    <v>0</v>
+    <v>Image of New South Wales</v>
+  </rv>
+  <rv s="0">
+    <v>805306368</v>
+    <v>Charles III (Monarch)</v>
+    <v>afc6f6a9-5b55-9178-3e6f-2c8b6d16ee9c</v>
+    <v>en-AU</v>
+    <v>Generic</v>
+  </rv>
+  <rv s="0">
+    <v>805306368</v>
+    <v>Margaret Beazley (Governor)</v>
+    <v>1d8fb294-de91-9fc8-2dc7-475add710304</v>
+    <v>en-AU</v>
+    <v>Generic</v>
+  </rv>
+  <rv s="0">
+    <v>805306368</v>
+    <v>Chris Minns (Premier)</v>
+    <v>0778fbcf-e8a7-bb64-039c-8e30d13c2fc3</v>
+    <v>en-AU</v>
+    <v>Generic</v>
+  </rv>
+  <rv s="3">
+    <v>0</v>
+  </rv>
+  <rv s="4">
+    <v>https://www.bing.com/search?q=new+south+wales&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <fb>1647</fb>
+    <v>12</v>
+  </rv>
+  <rv s="1">
+    <fb>77272</fb>
+    <v>12</v>
+  </rv>
+  <rv s="1">
+    <fb>2.6</fb>
+    <v>13</v>
+  </rv>
+  <rv s="1">
+    <fb>8157735</fb>
+    <v>11</v>
+  </rv>
+  <rv s="1">
+    <fb>1.6E-2</fb>
+    <v>14</v>
+  </rv>
+  <rv s="5">
+    <v>#VALUE!</v>
+    <v>en-AU</v>
+    <v>9143b1e4-782f-52c3-0f4a-cea5eaf6f36a</v>
+    <v>536870912</v>
+    <v>1</v>
+    <v>4</v>
+    <v>5</v>
+    <v>New South Wales</v>
+    <v>7</v>
+    <v>8</v>
+    <v>Map</v>
+    <v>9</v>
+    <v>10</v>
+    <v>AU-NSW</v>
+    <v>1</v>
+    <v>2</v>
+    <v>3</v>
+    <v>New South Wales is a state on the east coast of Australia. It borders Queensland to the north, Victoria to the south, and South Australia to the west. Its coast borders the Coral and Tasman Seas to the east. The Australian Capital Territory and ...</v>
+    <v>4</v>
+    <v>4</v>
+    <v>5</v>
+    <v>2</v>
+    <v>9</v>
+    <v>10</v>
+    <v>11</v>
+    <v>12</v>
+    <v>New South Wales</v>
+    <v>13</v>
+    <v>14</v>
+    <v>15</v>
+    <v>New South Wales</v>
+    <v>mdp/vdpid/23155</v>
+  </rv>
+  <rv s="0">
+    <v>536870912</v>
+    <v>Victoria</v>
+    <v>afad25fd-4cbc-2e30-7764-19bd8a1cb1bc</v>
+    <v>en-AU</v>
+    <v>Map</v>
+  </rv>
+  <rv s="1">
+    <fb>227444</fb>
+    <v>11</v>
+  </rv>
+  <rv s="0">
+    <v>536870912</v>
+    <v>Melbourne</v>
+    <v>8b583bb3-5207-934d-55d1-8ab5089fd70e</v>
+    <v>en-AU</v>
+    <v>Map</v>
+  </rv>
+  <rv s="1">
+    <fb>2112706</fb>
+    <v>11</v>
+  </rv>
+  <rv s="2">
+    <v>1</v>
+    <v>9</v>
+    <v>15</v>
+    <v>7</v>
+    <v>0</v>
+    <v>Image of Victoria</v>
+  </rv>
+  <rv s="0">
+    <v>805306368</v>
+    <v>Margaret Gardner (Governor)</v>
+    <v>2a78d71a-cf4c-9647-da14-6790bd1d57e9</v>
+    <v>en-AU</v>
+    <v>Generic</v>
+  </rv>
+  <rv s="0">
+    <v>805306368</v>
+    <v>Daniel Andrews (Premier)</v>
+    <v>270ee44f-f743-4472-2e75-94103734eac1</v>
+    <v>en-AU</v>
+    <v>Generic</v>
+  </rv>
+  <rv s="3">
+    <v>1</v>
+  </rv>
+  <rv s="4">
+    <v>https://www.bing.com/search?q=victoria+australia&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <fb>1408</fb>
+    <v>12</v>
+  </rv>
+  <rv s="1">
+    <fb>73788</fb>
+    <v>12</v>
+  </rv>
+  <rv s="1">
+    <fb>6689377</fb>
+    <v>11</v>
+  </rv>
+  <rv s="1">
+    <fb>2.3E-2</fb>
+    <v>14</v>
+  </rv>
+  <rv s="5">
+    <v>#VALUE!</v>
+    <v>en-AU</v>
+    <v>afad25fd-4cbc-2e30-7764-19bd8a1cb1bc</v>
+    <v>536870912</v>
+    <v>1</v>
+    <v>19</v>
+    <v>5</v>
+    <v>Victoria</v>
+    <v>7</v>
+    <v>8</v>
+    <v>Map</v>
+    <v>9</v>
+    <v>10</v>
+    <v>AU-VIC</v>
+    <v>18</v>
+    <v>19</v>
+    <v>3</v>
+    <v>Victoria is a state in southeastern Australia. It is the second-smallest state, with a land area of 227,444 km² ; the second-most-populated state, with a population of over 6.7 million; and the most densely populated state in Australia. Victoria ...</v>
+    <v>20</v>
+    <v>20</v>
+    <v>21</v>
+    <v>19</v>
+    <v>24</v>
+    <v>25</v>
+    <v>26</v>
+    <v>27</v>
+    <v>Victoria</v>
+    <v>13</v>
+    <v>28</v>
+    <v>29</v>
+    <v>Victoria</v>
+    <v>mdp/vdpid/35121</v>
+  </rv>
+  <rv s="0">
+    <v>536870912</v>
+    <v>Queensland</v>
+    <v>d8d1c6ea-bc68-82f2-5bb3-ae7aa11442b4</v>
+    <v>en-AU</v>
+    <v>Map</v>
+  </rv>
+  <rv s="1">
+    <fb>1729742</fb>
+    <v>11</v>
+  </rv>
+  <rv s="0">
+    <v>536870912</v>
+    <v>Brisbane</v>
+    <v>42da5c6f-c43f-8401-d736-da01adb6e95c</v>
+    <v>en-AU</v>
+    <v>Map</v>
+  </rv>
+  <rv s="1">
+    <fb>1656831</fb>
+    <v>11</v>
+  </rv>
+  <rv s="2">
+    <v>2</v>
+    <v>9</v>
+    <v>20</v>
+    <v>7</v>
+    <v>0</v>
+    <v>Image of Queensland</v>
+  </rv>
+  <rv s="0">
+    <v>805306368</v>
+    <v>Jeannette Young (Governor)</v>
+    <v>b9266fb4-1992-87ff-1819-ae64a938c5e6</v>
+    <v>en-AU</v>
+    <v>Generic</v>
+  </rv>
+  <rv s="0">
+    <v>805306368</v>
+    <v>Annastacia Palaszczuk (Premier)</v>
+    <v>e47dc47b-0698-6175-67b3-e05a6ca083b2</v>
+    <v>en-AU</v>
+    <v>Generic</v>
+  </rv>
+  <rv s="3">
+    <v>2</v>
+  </rv>
+  <rv s="4">
+    <v>https://www.bing.com/search?q=queensland+australia&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <fb>1430</fb>
+    <v>12</v>
+  </rv>
+  <rv s="1">
+    <fb>72904</fb>
+    <v>12</v>
+  </rv>
+  <rv s="1">
+    <fb>5160023</fb>
+    <v>11</v>
+  </rv>
+  <rv s="5">
+    <v>#VALUE!</v>
+    <v>en-AU</v>
+    <v>d8d1c6ea-bc68-82f2-5bb3-ae7aa11442b4</v>
+    <v>536870912</v>
+    <v>1</v>
+    <v>24</v>
+    <v>5</v>
+    <v>Queensland</v>
+    <v>7</v>
+    <v>8</v>
+    <v>Map</v>
+    <v>9</v>
+    <v>10</v>
+    <v>AU-QLD</v>
+    <v>32</v>
+    <v>33</v>
+    <v>3</v>
+    <v>Queensland is a state situated in northeastern Australia, and is the second-largest and third-most populous of the Australian states. It is bordered by the Northern Territory, South Australia and New South Wales to the west, southwest and south ...</v>
+    <v>34</v>
+    <v>34</v>
+    <v>35</v>
+    <v>33</v>
+    <v>38</v>
+    <v>39</v>
+    <v>40</v>
+    <v>41</v>
+    <v>Queensland</v>
+    <v>13</v>
+    <v>42</v>
+    <v>15</v>
+    <v>Queensland</v>
+    <v>mdp/vdpid/27085</v>
+  </rv>
+  <rv s="0">
+    <v>536870912</v>
+    <v>Western Australia</v>
+    <v>bf87c7cd-72cb-99af-809b-eb7577149dcd</v>
+    <v>en-AU</v>
+    <v>Map</v>
+  </rv>
+  <rv s="1">
+    <fb>2527013</fb>
+    <v>11</v>
+  </rv>
+  <rv s="0">
+    <v>536870912</v>
+    <v>Perth</v>
+    <v>0cba98f1-710c-4d9f-a96f-b5f737acde07</v>
+    <v>en-AU</v>
+    <v>Map</v>
+  </rv>
+  <rv s="1">
+    <fb>866777</fb>
+    <v>11</v>
+  </rv>
+  <rv s="2">
+    <v>3</v>
+    <v>9</v>
+    <v>25</v>
+    <v>7</v>
+    <v>0</v>
+    <v>Image of Western Australia</v>
+  </rv>
+  <rv s="0">
+    <v>805306368</v>
+    <v>Chris Dawson (Governor)</v>
+    <v>d733e039-cda3-4744-e7fd-82f729a3b565</v>
+    <v>en-AU</v>
+    <v>Generic</v>
+  </rv>
+  <rv s="0">
+    <v>805306368</v>
+    <v>Roger Cook (Premier)</v>
+    <v>c862c3c1-464f-67e8-fdb7-9e813eef2e77</v>
+    <v>en-AU</v>
+    <v>Generic</v>
+  </rv>
+  <rv s="3">
+    <v>3</v>
+  </rv>
+  <rv s="4">
+    <v>https://www.bing.com/search?q=western+australia&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <fb>1504</fb>
+    <v>12</v>
+  </rv>
+  <rv s="1">
+    <fb>82940</fb>
+    <v>12</v>
+  </rv>
+  <rv s="1">
+    <fb>2656156</fb>
+    <v>11</v>
+  </rv>
+  <rv s="1">
+    <fb>8.0000000000000002E-3</fb>
+    <v>14</v>
+  </rv>
+  <rv s="5">
+    <v>#VALUE!</v>
+    <v>en-AU</v>
+    <v>bf87c7cd-72cb-99af-809b-eb7577149dcd</v>
+    <v>536870912</v>
+    <v>1</v>
+    <v>29</v>
+    <v>5</v>
+    <v>Western Australia</v>
+    <v>7</v>
+    <v>8</v>
+    <v>Map</v>
+    <v>9</v>
+    <v>10</v>
+    <v>AU-WA</v>
+    <v>45</v>
+    <v>46</v>
+    <v>3</v>
+    <v>Western Australia is a state of Australia occupying the western 33 percent of the land area of Australia, excluding external territories. It is bounded by the Indian Ocean to the north and west, the Southern Ocean to the south, the Northern ...</v>
+    <v>47</v>
+    <v>47</v>
+    <v>48</v>
+    <v>46</v>
+    <v>51</v>
+    <v>52</v>
+    <v>53</v>
+    <v>54</v>
+    <v>Western Australia</v>
+    <v>13</v>
+    <v>55</v>
+    <v>56</v>
+    <v>Western Australia</v>
+    <v>mdp/vdpid/36233</v>
+  </rv>
+  <rv s="0">
+    <v>536870912</v>
+    <v>South Australia</v>
+    <v>202994ba-49c2-98c5-91fa-e0b05ffcf2da</v>
+    <v>en-AU</v>
+    <v>Map</v>
+  </rv>
+  <rv s="1">
+    <fb>984321</fb>
+    <v>11</v>
+  </rv>
+  <rv s="0">
+    <v>536870912</v>
+    <v>Adelaide</v>
+    <v>846dc96e-cf3d-6f5f-295b-2ec458ee2963</v>
+    <v>en-AU</v>
+    <v>Map</v>
+  </rv>
+  <rv s="0">
+    <v>536870912</v>
+    <v>United Kingdom of Great Britain and Ireland</v>
+    <v>0538d165-f2b4-64c9-9745-179dd804d95b</v>
+    <v>en-AU</v>
+    <v>Map</v>
+  </rv>
+  <rv s="1">
+    <fb>638792</fb>
+    <v>11</v>
+  </rv>
+  <rv s="2">
+    <v>4</v>
+    <v>9</v>
+    <v>30</v>
+    <v>7</v>
+    <v>0</v>
+    <v>Image of South Australia</v>
+  </rv>
+  <rv s="0">
+    <v>805306368</v>
+    <v>Frances Adamson (Governor)</v>
+    <v>2e49d47b-17ab-515d-c4ff-129324a5e635</v>
+    <v>en-AU</v>
+    <v>Generic</v>
+  </rv>
+  <rv s="0">
+    <v>805306368</v>
+    <v>Peter Malinauskas (Premier)</v>
+    <v>a636f18e-e52f-cf74-63ee-caf593cdbdf4</v>
+    <v>en-AU</v>
+    <v>Generic</v>
+  </rv>
+  <rv s="3">
+    <v>4</v>
+  </rv>
+  <rv s="4">
+    <v>https://www.bing.com/search?q=south+australia&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <fb>1127</fb>
+    <v>12</v>
+  </rv>
+  <rv s="1">
+    <fb>62712</fb>
+    <v>12</v>
+  </rv>
+  <rv s="1">
+    <fb>2.4</fb>
+    <v>13</v>
+  </rv>
+  <rv s="1">
+    <fb>1767247</fb>
+    <v>11</v>
+  </rv>
+  <rv s="1">
+    <fb>6.0000000000000001E-3</fb>
+    <v>14</v>
+  </rv>
+  <rv s="5">
+    <v>#VALUE!</v>
+    <v>en-AU</v>
+    <v>202994ba-49c2-98c5-91fa-e0b05ffcf2da</v>
+    <v>536870912</v>
+    <v>1</v>
+    <v>34</v>
+    <v>5</v>
+    <v>South Australia</v>
+    <v>7</v>
+    <v>8</v>
+    <v>Map</v>
+    <v>9</v>
+    <v>10</v>
+    <v>AU-SA</v>
+    <v>59</v>
+    <v>60</v>
+    <v>61</v>
+    <v>South Australia is a state in the southern central part of Australia. It covers some of the most arid parts of the country. With a total land area of 984,321 square kilometres, it is the fourth-largest of Australia's states and territories by ...</v>
+    <v>62</v>
+    <v>62</v>
+    <v>63</v>
+    <v>60</v>
+    <v>66</v>
+    <v>67</v>
+    <v>68</v>
+    <v>69</v>
+    <v>South Australia</v>
+    <v>70</v>
+    <v>71</v>
+    <v>72</v>
+    <v>South Australia</v>
+    <v>mdp/vdpid/31398</v>
+  </rv>
+  <rv s="0">
+    <v>536870912</v>
+    <v>Tasmania</v>
+    <v>8327961c-5e1c-9007-38cc-b90bc76e7bc3</v>
+    <v>en-AU</v>
+    <v>Map</v>
+  </rv>
+  <rv s="1">
+    <fb>68401</fb>
+    <v>11</v>
+  </rv>
+  <rv s="0">
+    <v>536870912</v>
+    <v>Hobart</v>
+    <v>5b31c3a7-a227-3016-652e-c7dea37e9068</v>
+    <v>en-AU</v>
+    <v>Map</v>
+  </rv>
+  <rv s="1">
+    <fb>197575</fb>
+    <v>11</v>
+  </rv>
+  <rv s="2">
+    <v>5</v>
+    <v>9</v>
+    <v>35</v>
+    <v>7</v>
+    <v>0</v>
+    <v>Image of Tasmania</v>
+  </rv>
+  <rv s="0">
+    <v>805306368</v>
+    <v>Barbara Baker (Governor)</v>
+    <v>7070225b-f22d-fbde-92c4-e4316f09de22</v>
+    <v>en-AU</v>
+    <v>Generic</v>
+  </rv>
+  <rv s="0">
+    <v>805306368</v>
+    <v>Jeremy Rockliff (Premier)</v>
+    <v>fd0473ab-30a2-45e6-d9b4-0ef9c550cecd</v>
+    <v>en-AU</v>
+    <v>Generic</v>
+  </rv>
+  <rv s="3">
+    <v>5</v>
+  </rv>
+  <rv s="4">
+    <v>https://www.bing.com/search?q=tasmania&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <fb>997</fb>
+    <v>12</v>
+  </rv>
+  <rv s="1">
+    <fb>57200</fb>
+    <v>12</v>
+  </rv>
+  <rv s="1">
+    <fb>2.2999999999999998</fb>
+    <v>13</v>
+  </rv>
+  <rv s="1">
+    <fb>539590</fb>
+    <v>11</v>
+  </rv>
+  <rv s="5">
+    <v>#VALUE!</v>
+    <v>en-AU</v>
+    <v>8327961c-5e1c-9007-38cc-b90bc76e7bc3</v>
+    <v>536870912</v>
+    <v>1</v>
+    <v>39</v>
+    <v>5</v>
+    <v>Tasmania</v>
+    <v>7</v>
+    <v>8</v>
+    <v>Map</v>
+    <v>9</v>
+    <v>10</v>
+    <v>AU-TAS</v>
+    <v>75</v>
+    <v>76</v>
+    <v>3</v>
+    <v>Tasmania is an island state of Australia. It is located 240 kilometres to the south of the Australian mainland, separated from it by the Bass Strait, with the archipelago containing the southernmost point of the country. The state encompasses ...</v>
+    <v>77</v>
+    <v>77</v>
+    <v>78</v>
+    <v>76</v>
+    <v>81</v>
+    <v>82</v>
+    <v>83</v>
+    <v>84</v>
+    <v>Tasmania</v>
+    <v>85</v>
+    <v>86</v>
+    <v>72</v>
+    <v>Tasmania</v>
+    <v>mdp/vdpid/32840</v>
+  </rv>
+  <rv s="0">
+    <v>536870912</v>
+    <v>Australian Capital Territory</v>
+    <v>c296eb2e-2c1a-16bf-bc37-164541ce7365</v>
+    <v>en-AU</v>
+    <v>Map</v>
+  </rv>
+  <rv s="1">
+    <fb>2358</fb>
+    <v>11</v>
+  </rv>
+  <rv s="0">
+    <v>536870912</v>
+    <v>Canberra</v>
+    <v>59ab58e3-2f00-9175-e7b8-76d910040855</v>
+    <v>en-AU</v>
+    <v>Map</v>
+  </rv>
+  <rv s="1">
+    <fb>142664</fb>
+    <v>11</v>
+  </rv>
+  <rv s="2">
+    <v>6</v>
+    <v>9</v>
+    <v>40</v>
+    <v>7</v>
+    <v>0</v>
+    <v>Image of Australian Capital Territory</v>
+  </rv>
+  <rv s="0">
+    <v>805306368</v>
+    <v>Andrew Barr (Chief minister)</v>
+    <v>292fe674-023a-df11-cc87-947ddb449aaf</v>
+    <v>en-AU</v>
+    <v>Generic</v>
+  </rv>
+  <rv s="3">
+    <v>6</v>
+  </rv>
+  <rv s="4">
+    <v>https://www.bing.com/search?q=australian+capital+territory&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <fb>107640</fb>
+    <v>12</v>
+  </rv>
+  <rv s="1">
+    <fb>2.5</fb>
+    <v>13</v>
+  </rv>
+  <rv s="1">
+    <fb>429834</fb>
+    <v>11</v>
+  </rv>
+  <rv s="1">
+    <fb>1.7000000000000001E-2</fb>
+    <v>14</v>
+  </rv>
+  <rv s="5">
+    <v>#VALUE!</v>
+    <v>en-AU</v>
+    <v>c296eb2e-2c1a-16bf-bc37-164541ce7365</v>
+    <v>536870912</v>
+    <v>1</v>
+    <v>44</v>
+    <v>5</v>
+    <v>Australian Capital Territory</v>
+    <v>7</v>
+    <v>8</v>
+    <v>Map</v>
+    <v>9</v>
+    <v>10</v>
+    <v>AU-ACT</v>
+    <v>89</v>
+    <v>90</v>
+    <v>3</v>
+    <v>The Australian Capital Territory, known as the Federal Capital Territory until 1938, is a federal territory of Australia. Canberra, the capital city of Australia, is located in this territory. It is located in southeastern Australian mainland as ...</v>
+    <v>91</v>
+    <v>91</v>
+    <v>92</v>
+    <v>90</v>
+    <v>94</v>
+    <v>95</v>
+    <v>11</v>
+    <v>96</v>
+    <v>Australian Capital Territory</v>
+    <v>97</v>
+    <v>98</v>
+    <v>99</v>
+    <v>Australian Capital Territory</v>
+    <v>mdp/vdpid/2353</v>
+  </rv>
+  <rv s="0">
+    <v>536870912</v>
+    <v>Northern Territory</v>
+    <v>20947ace-4dd4-0516-21df-2af8da517b06</v>
+    <v>en-AU</v>
+    <v>Map</v>
+  </rv>
+  <rv s="1">
+    <fb>1347791</fb>
+    <v>11</v>
+  </rv>
+  <rv s="0">
+    <v>536870912</v>
+    <v>Darwin</v>
+    <v>8d773b06-b293-eac0-d743-3ebe93419aca</v>
+    <v>en-AU</v>
+    <v>Map</v>
+  </rv>
+  <rv s="1">
+    <fb>65061</fb>
+    <v>11</v>
+  </rv>
+  <rv s="2">
+    <v>7</v>
+    <v>9</v>
+    <v>45</v>
+    <v>7</v>
+    <v>0</v>
+    <v>Image of Northern Territory</v>
+  </rv>
+  <rv s="0">
+    <v>805306368</v>
+    <v>Natasha Fyles (Chief minister)</v>
+    <v>0548a54d-3d0f-48c0-8f43-035060c86da2</v>
+    <v>en-AU</v>
+    <v>Generic</v>
+  </rv>
+  <rv s="3">
+    <v>7</v>
+  </rv>
+  <rv s="4">
+    <v>https://www.bing.com/search?q=northern+territory&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <fb>1365</fb>
+    <v>12</v>
+  </rv>
+  <rv s="1">
+    <fb>103116</fb>
+    <v>12</v>
+  </rv>
+  <rv s="1">
+    <fb>2.9</fb>
+    <v>13</v>
+  </rv>
+  <rv s="1">
+    <fb>245353</fb>
+    <v>11</v>
+  </rv>
+  <rv s="1">
+    <fb>1E-3</fb>
+    <v>14</v>
+  </rv>
+  <rv s="5">
+    <v>#VALUE!</v>
+    <v>en-AU</v>
+    <v>20947ace-4dd4-0516-21df-2af8da517b06</v>
+    <v>536870912</v>
+    <v>1</v>
+    <v>49</v>
+    <v>5</v>
+    <v>Northern Territory</v>
+    <v>7</v>
+    <v>8</v>
+    <v>Map</v>
+    <v>9</v>
+    <v>10</v>
+    <v>AU-NT</v>
+    <v>102</v>
+    <v>103</v>
+    <v>3</v>
+    <v>The Northern Territory is an Australian territory in the central and central northern regions of Australia. The Northern Territory shares its borders with Western Australia to the west, South Australia to the south, and Queensland to the east. ...</v>
+    <v>104</v>
+    <v>104</v>
+    <v>105</v>
+    <v>103</v>
+    <v>107</v>
+    <v>108</v>
+    <v>109</v>
+    <v>110</v>
+    <v>Northern Territory</v>
+    <v>111</v>
+    <v>112</v>
+    <v>113</v>
+    <v>Northern Territory</v>
+    <v>mdp/vdpid/23745</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="6">
+  <s t="_linkedentity2">
+    <k n="%EntityServiceId" t="i"/>
+    <k n="_DisplayString" t="s"/>
+    <k n="%EntityId" t="s"/>
+    <k n="%EntityCulture" t="s"/>
+    <k n="_Icon" t="s"/>
+  </s>
+  <s t="_formattednumber">
+    <k n="_Format" t="spb"/>
+  </s>
+  <s t="_webimage">
+    <k n="WebImageIdentifier" t="i"/>
+    <k n="_Provider" t="spb"/>
+    <k n="Attribution" t="spb"/>
+    <k n="CalcOrigin" t="i"/>
+    <k n="ComputedImage" t="b"/>
+    <k n="Text" t="s"/>
+  </s>
+  <s t="_array">
+    <k n="array" t="a"/>
+  </s>
+  <s t="_hyperlink">
+    <k n="Address" t="s"/>
+    <k n="Text" t="s"/>
+  </s>
+  <s t="_linkedentity2core">
+    <k n="_CRID" t="e"/>
+    <k n="%EntityCulture" t="s"/>
+    <k n="%EntityId" t="s"/>
+    <k n="%EntityServiceId" t="i"/>
+    <k n="%IsRefreshable" t="b"/>
+    <k n="_Attribution" t="spb"/>
+    <k n="_Display" t="spb"/>
+    <k n="_DisplayString" t="s"/>
+    <k n="_Flags" t="spb"/>
+    <k n="_Format" t="spb"/>
+    <k n="_Icon" t="s"/>
+    <k n="_Provider" t="spb"/>
+    <k n="_SubLabel" t="spb"/>
+    <k n="Abbreviation" t="s"/>
+    <k n="Area" t="r"/>
+    <k n="Capital/Major City" t="r"/>
+    <k n="Country/region" t="r"/>
+    <k n="Description" t="s"/>
+    <k n="Households" t="r"/>
+    <k n="Housing units" t="r"/>
+    <k n="Image" t="r"/>
+    <k n="Largest city" t="r"/>
+    <k n="Leader(s)" t="r"/>
+    <k n="LearnMoreOnLink" t="r"/>
+    <k n="Median gross rent" t="r"/>
+    <k n="Median household income" t="r"/>
+    <k n="Name" t="s"/>
+    <k n="Persons per household" t="r"/>
+    <k n="Population" t="r"/>
+    <k n="Population change (%)" t="r"/>
+    <k n="UniqueName" t="s"/>
+    <k n="VDPID/VSID" t="s"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
+<supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
+  <spbArrays count="1">
+    <a count="31">
+      <v t="s">%EntityServiceId</v>
+      <v t="s">%IsRefreshable</v>
+      <v t="s">%EntityCulture</v>
+      <v t="s">%EntityId</v>
+      <v t="s">_Icon</v>
+      <v t="s">_Provider</v>
+      <v t="s">_Attribution</v>
+      <v t="s">_Display</v>
+      <v t="s">Name</v>
+      <v t="s">_Format</v>
+      <v t="s">Capital/Major City</v>
+      <v t="s">Leader(s)</v>
+      <v t="s">Country/region</v>
+      <v t="s">_SubLabel</v>
+      <v t="s">Population</v>
+      <v t="s">Area</v>
+      <v t="s">Abbreviation</v>
+      <v t="s">Largest city</v>
+      <v t="s">Population change (%)</v>
+      <v t="s">Households</v>
+      <v t="s">Housing units</v>
+      <v t="s">Persons per household</v>
+      <v t="s">Median household income</v>
+      <v t="s">Median gross rent</v>
+      <v t="s">_Flags</v>
+      <v t="s">VDPID/VSID</v>
+      <v t="s">UniqueName</v>
+      <v t="s">_DisplayString</v>
+      <v t="s">LearnMoreOnLink</v>
+      <v t="s">Image</v>
+      <v t="s">Description</v>
+    </a>
+  </spbArrays>
+  <spbData count="50">
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	</v>
+      <v xml:space="preserve">CC BY-SA 3.0	</v>
+      <v xml:space="preserve">https://en.wikipedia.org/wiki/New_South_Wales	</v>
+      <v xml:space="preserve">https://creativecommons.org/licenses/by-sa/3.0	</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Britannica	</v>
+      <v xml:space="preserve">	</v>
+      <v xml:space="preserve">https://www.britannica.com/place/New-South-Wales	</v>
+      <v xml:space="preserve">	</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	</v>
+      <v xml:space="preserve">CC-BY-SA	</v>
+      <v xml:space="preserve">http://en.wikipedia.org/wiki/New_South_Wales	</v>
+      <v xml:space="preserve">http://creativecommons.org/licenses/by-sa/3.0/	</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	Britannica	</v>
+      <v xml:space="preserve">CC-BY-SA		</v>
+      <v xml:space="preserve">http://en.wikipedia.org/wiki/New_South_Wales	https://www.britannica.com/place/New-South-Wales	</v>
+      <v xml:space="preserve">http://creativecommons.org/licenses/by-sa/3.0/		</v>
+    </spb>
+    <spb s="1">
+      <v>0</v>
+      <v>0</v>
+      <v>1</v>
+      <v>0</v>
+      <v>0</v>
+      <v>0</v>
+      <v>2</v>
+      <v>0</v>
+      <v>1</v>
+      <v>0</v>
+      <v>3</v>
+      <v>0</v>
+      <v>1</v>
+      <v>1</v>
+      <v>3</v>
+    </spb>
+    <spb s="2">
+      <v>0</v>
+      <v>Name</v>
+      <v>LearnMoreOnLink</v>
+    </spb>
+    <spb s="3">
+      <v>0</v>
+      <v>0</v>
+      <v>0</v>
+    </spb>
+    <spb s="4">
+      <v>6</v>
+      <v>6</v>
+      <v>6</v>
+    </spb>
+    <spb s="5">
+      <v>1</v>
+      <v>2</v>
+    </spb>
+    <spb s="6">
+      <v>https://www.bing.com</v>
+      <v>https://www.bing.com/th?id=Ga%5Cbing_yt.png&amp;w=100&amp;h=40&amp;c=0&amp;pid=0.1</v>
+      <v>Powered by Bing</v>
+    </spb>
+    <spb s="7">
+      <v>square km</v>
+      <v>2016</v>
+      <v>2020</v>
+      <v>2016</v>
+      <v>2016</v>
+      <v>2016</v>
+      <v>2016, 2017</v>
+      <v>2016</v>
+    </spb>
+    <spb s="8">
+      <v>3</v>
+    </spb>
+    <spb s="8">
+      <v>4</v>
+    </spb>
+    <spb s="8">
+      <v>5</v>
+    </spb>
+    <spb s="8">
+      <v>6</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	</v>
+      <v xml:space="preserve">CC BY-SA 3.0	</v>
+      <v xml:space="preserve">https://en.wikipedia.org/wiki/Victoria_(state)	</v>
+      <v xml:space="preserve">https://creativecommons.org/licenses/by-sa/3.0	</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	</v>
+      <v xml:space="preserve">CC-BY-SA	</v>
+      <v xml:space="preserve">https://en.wikipedia.org/wiki/Victoria_(Australia)	</v>
+      <v xml:space="preserve">http://creativecommons.org/licenses/by-sa/3.0/	</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	</v>
+      <v xml:space="preserve">CC-BY-SA	</v>
+      <v xml:space="preserve">http://en.wikipedia.org/wiki/Victoria_(Australia)	</v>
+      <v xml:space="preserve">http://creativecommons.org/licenses/by-sa/3.0/	</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	Wikipedia	</v>
+      <v xml:space="preserve">CC-BY-SA	CC-BY-SA	</v>
+      <v xml:space="preserve">http://en.wikipedia.org/wiki/Victoria_(Australia)	https://en.wikipedia.org/wiki/Victoria_(Australia)	</v>
+      <v xml:space="preserve">http://creativecommons.org/licenses/by-sa/3.0/	http://creativecommons.org/licenses/by-sa/3.0/	</v>
+    </spb>
+    <spb s="1">
+      <v>15</v>
+      <v>15</v>
+      <v>16</v>
+      <v>15</v>
+      <v>15</v>
+      <v>15</v>
+      <v>17</v>
+      <v>15</v>
+      <v>16</v>
+      <v>15</v>
+      <v>18</v>
+      <v>15</v>
+      <v>16</v>
+      <v>16</v>
+      <v>18</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	</v>
+      <v xml:space="preserve">CC BY-SA 3.0	</v>
+      <v xml:space="preserve">https://en.wikipedia.org/wiki/Queensland	</v>
+      <v xml:space="preserve">https://creativecommons.org/licenses/by-sa/3.0	</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	</v>
+      <v xml:space="preserve">CC-BY-SA	</v>
+      <v xml:space="preserve">https://en.wikipedia.org/wiki/Queensland	</v>
+      <v xml:space="preserve">http://creativecommons.org/licenses/by-sa/3.0/	</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	</v>
+      <v xml:space="preserve">CC-BY-SA	</v>
+      <v xml:space="preserve">http://en.wikipedia.org/wiki/Queensland	</v>
+      <v xml:space="preserve">http://creativecommons.org/licenses/by-sa/3.0/	</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	Wikipedia	</v>
+      <v xml:space="preserve">CC-BY-SA	CC-BY-SA	</v>
+      <v xml:space="preserve">http://en.wikipedia.org/wiki/Queensland	https://en.wikipedia.org/wiki/Queensland	</v>
+      <v xml:space="preserve">http://creativecommons.org/licenses/by-sa/3.0/	http://creativecommons.org/licenses/by-sa/3.0/	</v>
+    </spb>
+    <spb s="1">
+      <v>20</v>
+      <v>20</v>
+      <v>21</v>
+      <v>20</v>
+      <v>20</v>
+      <v>20</v>
+      <v>22</v>
+      <v>20</v>
+      <v>21</v>
+      <v>20</v>
+      <v>23</v>
+      <v>20</v>
+      <v>21</v>
+      <v>21</v>
+      <v>23</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	</v>
+      <v xml:space="preserve">CC BY-SA 3.0	</v>
+      <v xml:space="preserve">https://en.wikipedia.org/wiki/Western_Australia	</v>
+      <v xml:space="preserve">https://creativecommons.org/licenses/by-sa/3.0	</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	</v>
+      <v xml:space="preserve">CC-BY-SA	</v>
+      <v xml:space="preserve">https://en.wikipedia.org/wiki/Western_Australia	</v>
+      <v xml:space="preserve">http://creativecommons.org/licenses/by-sa/3.0/	</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	</v>
+      <v xml:space="preserve">CC-BY-SA	</v>
+      <v xml:space="preserve">http://en.wikipedia.org/wiki/Western_Australia	</v>
+      <v xml:space="preserve">http://creativecommons.org/licenses/by-sa/3.0/	</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	Wikipedia	</v>
+      <v xml:space="preserve">CC-BY-SA	CC-BY-SA	</v>
+      <v xml:space="preserve">http://en.wikipedia.org/wiki/Western_Australia	https://en.wikipedia.org/wiki/Western_Australia	</v>
+      <v xml:space="preserve">http://creativecommons.org/licenses/by-sa/3.0/	http://creativecommons.org/licenses/by-sa/3.0/	</v>
+    </spb>
+    <spb s="1">
+      <v>25</v>
+      <v>25</v>
+      <v>26</v>
+      <v>25</v>
+      <v>25</v>
+      <v>25</v>
+      <v>27</v>
+      <v>25</v>
+      <v>26</v>
+      <v>25</v>
+      <v>28</v>
+      <v>25</v>
+      <v>26</v>
+      <v>26</v>
+      <v>28</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	</v>
+      <v xml:space="preserve">CC BY-SA 3.0	</v>
+      <v xml:space="preserve">https://en.wikipedia.org/wiki/South_Australia	</v>
+      <v xml:space="preserve">https://creativecommons.org/licenses/by-sa/3.0	</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Britannica	</v>
+      <v xml:space="preserve">	</v>
+      <v xml:space="preserve">https://www.britannica.com/place/South-Australia	</v>
+      <v xml:space="preserve">	</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	</v>
+      <v xml:space="preserve">CC-BY-SA	</v>
+      <v xml:space="preserve">http://en.wikipedia.org/wiki/South_Australia	</v>
+      <v xml:space="preserve">http://creativecommons.org/licenses/by-sa/3.0/	</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	Britannica	</v>
+      <v xml:space="preserve">CC-BY-SA		</v>
+      <v xml:space="preserve">http://en.wikipedia.org/wiki/South_Australia	https://www.britannica.com/place/South-Australia	</v>
+      <v xml:space="preserve">http://creativecommons.org/licenses/by-sa/3.0/		</v>
+    </spb>
+    <spb s="1">
+      <v>30</v>
+      <v>30</v>
+      <v>31</v>
+      <v>30</v>
+      <v>30</v>
+      <v>30</v>
+      <v>32</v>
+      <v>30</v>
+      <v>31</v>
+      <v>30</v>
+      <v>33</v>
+      <v>30</v>
+      <v>31</v>
+      <v>31</v>
+      <v>33</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	</v>
+      <v xml:space="preserve">CC BY-SA 3.0	</v>
+      <v xml:space="preserve">https://en.wikipedia.org/wiki/Tasmania	</v>
+      <v xml:space="preserve">https://creativecommons.org/licenses/by-sa/3.0	</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Britannica	</v>
+      <v xml:space="preserve">	</v>
+      <v xml:space="preserve">https://www.britannica.com/place/Tasmania	</v>
+      <v xml:space="preserve">	</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	</v>
+      <v xml:space="preserve">CC-BY-SA	</v>
+      <v xml:space="preserve">http://en.wikipedia.org/wiki/Tasmania	</v>
+      <v xml:space="preserve">http://creativecommons.org/licenses/by-sa/3.0/	</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	Britannica	</v>
+      <v xml:space="preserve">CC-BY-SA		</v>
+      <v xml:space="preserve">http://en.wikipedia.org/wiki/Tasmania	https://www.britannica.com/place/Tasmania	</v>
+      <v xml:space="preserve">http://creativecommons.org/licenses/by-sa/3.0/		</v>
+    </spb>
+    <spb s="1">
+      <v>35</v>
+      <v>35</v>
+      <v>36</v>
+      <v>35</v>
+      <v>35</v>
+      <v>35</v>
+      <v>37</v>
+      <v>35</v>
+      <v>36</v>
+      <v>35</v>
+      <v>38</v>
+      <v>35</v>
+      <v>36</v>
+      <v>36</v>
+      <v>38</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	</v>
+      <v xml:space="preserve">CC BY-SA 3.0	</v>
+      <v xml:space="preserve">https://en.wikipedia.org/wiki/Australian_Capital_Territory	</v>
+      <v xml:space="preserve">https://creativecommons.org/licenses/by-sa/3.0	</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Britannica	</v>
+      <v xml:space="preserve">	</v>
+      <v xml:space="preserve">https://www.britannica.com/place/Australian-Capital-Territory	</v>
+      <v xml:space="preserve">	</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	</v>
+      <v xml:space="preserve">CC-BY-SA	</v>
+      <v xml:space="preserve">http://en.wikipedia.org/wiki/Australian_Capital_Territory	</v>
+      <v xml:space="preserve">http://creativecommons.org/licenses/by-sa/3.0/	</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	Britannica	</v>
+      <v xml:space="preserve">CC-BY-SA		</v>
+      <v xml:space="preserve">http://en.wikipedia.org/wiki/Australian_Capital_Territory	https://www.britannica.com/place/Australian-Capital-Territory	</v>
+      <v xml:space="preserve">http://creativecommons.org/licenses/by-sa/3.0/		</v>
+    </spb>
+    <spb s="1">
+      <v>40</v>
+      <v>40</v>
+      <v>41</v>
+      <v>40</v>
+      <v>40</v>
+      <v>40</v>
+      <v>42</v>
+      <v>40</v>
+      <v>41</v>
+      <v>40</v>
+      <v>43</v>
+      <v>40</v>
+      <v>41</v>
+      <v>41</v>
+      <v>43</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	</v>
+      <v xml:space="preserve">CC BY-SA 3.0	</v>
+      <v xml:space="preserve">https://en.wikipedia.org/wiki/Northern_Territory	</v>
+      <v xml:space="preserve">https://creativecommons.org/licenses/by-sa/3.0	</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Britannica	</v>
+      <v xml:space="preserve">	</v>
+      <v xml:space="preserve">https://www.britannica.com/place/Northern-Territory	</v>
+      <v xml:space="preserve">	</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	</v>
+      <v xml:space="preserve">CC-BY-SA	</v>
+      <v xml:space="preserve">http://en.wikipedia.org/wiki/Northern_Territory	</v>
+      <v xml:space="preserve">http://creativecommons.org/licenses/by-sa/3.0/	</v>
+    </spb>
+    <spb s="0">
+      <v xml:space="preserve">Wikipedia	Britannica	</v>
+      <v xml:space="preserve">CC-BY-SA		</v>
+      <v xml:space="preserve">http://en.wikipedia.org/wiki/Northern_Territory	https://www.britannica.com/place/Northern-Territory	</v>
+      <v xml:space="preserve">http://creativecommons.org/licenses/by-sa/3.0/		</v>
+    </spb>
+    <spb s="1">
+      <v>45</v>
+      <v>45</v>
+      <v>46</v>
+      <v>45</v>
+      <v>45</v>
+      <v>45</v>
+      <v>47</v>
+      <v>45</v>
+      <v>46</v>
+      <v>45</v>
+      <v>48</v>
+      <v>45</v>
+      <v>46</v>
+      <v>46</v>
+      <v>48</v>
+    </spb>
+  </spbData>
+</supportingPropertyBags>
+</file>
+
+<file path=xl/richData/rdsupportingpropertybagstructure.xml><?xml version="1.0" encoding="utf-8"?>
+<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="9">
+  <s>
+    <k n="SourceText" t="s"/>
+    <k n="LicenseText" t="s"/>
+    <k n="SourceAddress" t="s"/>
+    <k n="LicenseAddress" t="s"/>
+  </s>
+  <s>
+    <k n="Area" t="spb"/>
+    <k n="Name" t="spb"/>
+    <k n="Households" t="spb"/>
+    <k n="Population" t="spb"/>
+    <k n="UniqueName" t="spb"/>
+    <k n="Description" t="spb"/>
+    <k n="Abbreviation" t="spb"/>
+    <k n="Largest city" t="spb"/>
+    <k n="Housing units" t="spb"/>
+    <k n="Country/region" t="spb"/>
+    <k n="Median gross rent" t="spb"/>
+    <k n="Capital/Major City" t="spb"/>
+    <k n="Persons per household" t="spb"/>
+    <k n="Population change (%)" t="spb"/>
+    <k n="Median household income" t="spb"/>
+  </s>
+  <s>
+    <k n="^Order" t="spba"/>
+    <k n="TitleProperty" t="s"/>
+    <k n="SubTitleProperty" t="s"/>
+  </s>
+  <s>
+    <k n="ShowInCardView" t="b"/>
+    <k n="ShowInDotNotation" t="b"/>
+    <k n="ShowInAutoComplete" t="b"/>
+  </s>
+  <s>
+    <k n="UniqueName" t="spb"/>
+    <k n="VDPID/VSID" t="spb"/>
+    <k n="LearnMoreOnLink" t="spb"/>
+  </s>
+  <s>
+    <k n="Name" t="i"/>
+    <k n="Image" t="i"/>
+  </s>
+  <s>
+    <k n="link" t="s"/>
+    <k n="logo" t="s"/>
+    <k n="name" t="s"/>
+  </s>
+  <s>
+    <k n="Area" t="s"/>
+    <k n="Households" t="s"/>
+    <k n="Population" t="s"/>
+    <k n="Housing units" t="s"/>
+    <k n="Median gross rent" t="s"/>
+    <k n="Persons per household" t="s"/>
+    <k n="Population change (%)" t="s"/>
+    <k n="Median household income" t="s"/>
+  </s>
+  <s>
+    <k n="_Self" t="i"/>
+  </s>
+</spbStructures>
+</file>
+
+<file path=xl/richData/richStyles.xml><?xml version="1.0" encoding="utf-8"?>
+<richStyleSheet xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <dxfs count="4">
+    <x:dxf>
+      <x:numFmt numFmtId="3" formatCode="#,##0"/>
+    </x:dxf>
+    <x:dxf>
+      <x:numFmt numFmtId="14" formatCode="0.00%"/>
+    </x:dxf>
+    <x:dxf>
+      <x:numFmt numFmtId="2" formatCode="0.00"/>
+    </x:dxf>
+    <x:dxf>
+      <x:numFmt numFmtId="0" formatCode="General"/>
+    </x:dxf>
+  </dxfs>
+  <richProperties>
+    <rPr n="IsTitleField" t="b"/>
+    <rPr n="IsHeroField" t="b"/>
+    <rPr n="NumberFormat" t="s"/>
+  </richProperties>
+  <richStyles>
+    <rSty>
+      <rpv i="0">1</rpv>
+    </rSty>
+    <rSty>
+      <rpv i="1">1</rpv>
+    </rSty>
+    <rSty dxfid="0">
+      <rpv i="2">#,##0</rpv>
+    </rSty>
+    <rSty dxfid="3">
+      <rpv i="2">_-[$$-en-AU]* #,##0_-;-[$$-en-AU]* #,##0_-;_-[$$-en-AU]* "-"_-;_-@_-</rpv>
+    </rSty>
+    <rSty dxfid="2">
+      <rpv i="2">0.00</rpv>
+    </rSty>
+    <rSty dxfid="1">
+      <rpv i="2">0.0%</rpv>
+    </rSty>
+  </richStyles>
+</richStyleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1137,15 +2860,15 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="19.25" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.4140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="16.4140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="8.4140625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.25" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.9140625" style="2" bestFit="1" customWidth="1"/>
@@ -1154,127 +2877,127 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
+      <c r="A2" s="1" t="e" vm="1">
+        <v>#VALUE!</v>
       </c>
       <c r="B2" s="2">
         <v>2021</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>0.43553446788487177</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>0.4738246534451957</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
+      <c r="A3" s="1" t="e" vm="2">
+        <v>#VALUE!</v>
       </c>
       <c r="B3" s="2">
         <v>2021</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>0.23615141296107495</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>0.26644580629112863</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
+      <c r="A4" s="1" t="e" vm="3">
+        <v>#VALUE!</v>
       </c>
       <c r="B4" s="2">
         <v>2021</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>0.2046244738974721</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>0.17611542027543475</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
+      <c r="A5" s="1" t="e" vm="4">
+        <v>#VALUE!</v>
       </c>
       <c r="B5" s="2">
         <v>2021</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>5.793009698585732E-2</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>1.5784355849031002E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
+      <c r="A6" s="1" t="e" vm="5">
+        <v>#VALUE!</v>
       </c>
       <c r="B6" s="2">
         <v>2021</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>3.1709931247222441E-2</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>5.5754053503991319E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
+      <c r="A7" s="1" t="e" vm="6">
+        <v>#VALUE!</v>
       </c>
       <c r="B7" s="2">
         <v>2021</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>3.1239379917914934E-3</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>3.1093824201171389E-3</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
-        <v>0</v>
+      <c r="A8" s="1" t="e" vm="7">
+        <v>#VALUE!</v>
       </c>
       <c r="B8" s="2">
         <v>2021</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>5.3590568060021436E-4</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>8.7967255376404877E-3</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
+      <c r="A9" s="1" t="e" vm="8">
+        <v>#VALUE!</v>
       </c>
       <c r="B9" s="2">
         <v>2021</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>3.0298277259299924E-2</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>1.1306845164062323E-5</v>
       </c>
     </row>

</xml_diff>